<commit_message>
MG: working in progress
</commit_message>
<xml_diff>
--- a/Coverage Survey/Madagascar/mg_cs_1_site.xlsx
+++ b/Coverage Survey/Madagascar/mg_cs_1_site.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\WHO\dsa-forms\Coverage Survey\Madagascar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B364AE71-C712-45D3-9CF7-1DAF0F7500FA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CB1DADA-7427-4F0D-AEEB-4283E3E8115D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="147">
   <si>
     <t>type</t>
   </si>
@@ -90,9 +90,6 @@
     <t>choice_filter</t>
   </si>
   <si>
-    <t>string</t>
-  </si>
-  <si>
     <t>date</t>
   </si>
   <si>
@@ -105,15 +102,9 @@
     <t>select_one site_ids</t>
   </si>
   <si>
-    <t>mg_cs_1_site</t>
-  </si>
-  <si>
     <t>French</t>
   </si>
   <si>
-    <t>1. Village</t>
-  </si>
-  <si>
     <t>label::French</t>
   </si>
   <si>
@@ -408,9 +399,6 @@
     <t>v_site_id</t>
   </si>
   <si>
-    <t>v_hh_vode</t>
-  </si>
-  <si>
     <t>v_interview_date</t>
   </si>
   <si>
@@ -435,9 +423,6 @@
     <t>Code Communauté</t>
   </si>
   <si>
-    <t>Code Ménage</t>
-  </si>
-  <si>
     <t>Date enquête</t>
   </si>
   <si>
@@ -472,6 +457,12 @@
   </si>
   <si>
     <t>Capturer les coordonnées géographiques</t>
+  </si>
+  <si>
+    <t>mg_cs_1_site_v2</t>
+  </si>
+  <si>
+    <t>1. Village V2</t>
   </si>
 </sst>
 </file>
@@ -882,10 +873,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -899,6 +890,7 @@
     <col min="7" max="7" width="36.7109375" customWidth="1"/>
     <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -909,10 +901,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>2</v>
@@ -921,7 +913,7 @@
         <v>3</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>4</v>
@@ -938,20 +930,20 @@
         <v>17</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="7" t="s">
         <v>18</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="H2" s="8"/>
       <c r="I2" s="8"/>
@@ -961,7 +953,7 @@
         <v>16</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>15</v>
@@ -980,10 +972,10 @@
         <v>20</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="7" t="s">
@@ -994,18 +986,18 @@
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
       <c r="J4" s="3" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="7" t="s">
@@ -1016,7 +1008,7 @@
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
       <c r="J5" s="3" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -1024,10 +1016,10 @@
         <v>22</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7" t="s">
@@ -1040,13 +1032,13 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="7" t="s">
@@ -1057,65 +1049,61 @@
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>17</v>
+        <v>141</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7" t="s">
-        <v>18</v>
-      </c>
+        <v>142</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
     </row>
-    <row r="9" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>146</v>
+        <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>148</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="D9" s="7"/>
       <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
-        <v>8</v>
+      <c r="A10" s="9" t="s">
+        <v>6</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
+        <v>128</v>
+      </c>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
       <c r="H10" s="8"/>
       <c r="I10" s="8"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
@@ -1126,22 +1114,7 @@
       <c r="I11" s="8"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B13" s="10"/>
+      <c r="B12" s="10"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>
@@ -1162,7 +1135,7 @@
   <dimension ref="A1:E263"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B184" sqref="B184"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1182,7 +1155,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>14</v>
@@ -1196,10 +1169,10 @@
         <v>14</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -1207,10 +1180,10 @@
         <v>14</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -1218,10 +1191,10 @@
         <v>14</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -1229,13 +1202,13 @@
         <v>19</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -1243,13 +1216,13 @@
         <v>19</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -1257,13 +1230,13 @@
         <v>19</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -1271,13 +1244,13 @@
         <v>19</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -1285,13 +1258,13 @@
         <v>19</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -1299,13 +1272,13 @@
         <v>19</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -1313,13 +1286,13 @@
         <v>19</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -1327,13 +1300,13 @@
         <v>19</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D12" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -1341,13 +1314,13 @@
         <v>19</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D13" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -1355,13 +1328,13 @@
         <v>19</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D14" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -1369,13 +1342,13 @@
         <v>19</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D15" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -1383,13 +1356,13 @@
         <v>19</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D16" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -1397,13 +1370,13 @@
         <v>19</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="D17" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -1411,13 +1384,13 @@
         <v>19</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="D18" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -1425,13 +1398,13 @@
         <v>19</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="D19" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -1439,13 +1412,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="D20" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -1453,13 +1426,13 @@
         <v>19</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="D21" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -1467,13 +1440,13 @@
         <v>19</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="D22" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -1481,13 +1454,13 @@
         <v>19</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D23" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -1495,13 +1468,13 @@
         <v>19</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="D24" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -1509,13 +1482,13 @@
         <v>19</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D25" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -1523,13 +1496,13 @@
         <v>19</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="D26" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -1537,13 +1510,13 @@
         <v>19</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="D27" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -1551,13 +1524,13 @@
         <v>19</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="D28" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -1565,13 +1538,13 @@
         <v>19</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="D29" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -1579,13 +1552,13 @@
         <v>19</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D30" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -1593,13 +1566,13 @@
         <v>19</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D31" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -1607,13 +1580,13 @@
         <v>19</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="D32" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -1621,13 +1594,13 @@
         <v>19</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="D33" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -1635,13 +1608,13 @@
         <v>19</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="D34" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -1649,13 +1622,13 @@
         <v>19</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D35" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -1663,13 +1636,13 @@
         <v>19</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D36" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -1677,13 +1650,13 @@
         <v>19</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D37" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -1691,13 +1664,13 @@
         <v>19</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="D38" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -1705,13 +1678,13 @@
         <v>19</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="D39" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
@@ -1719,13 +1692,13 @@
         <v>19</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="D40" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -1733,13 +1706,13 @@
         <v>19</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="D41" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
@@ -1747,13 +1720,13 @@
         <v>19</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D42" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -1761,13 +1734,13 @@
         <v>19</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="D43" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -1775,13 +1748,13 @@
         <v>19</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="D44" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
@@ -1789,13 +1762,13 @@
         <v>19</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D45" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -1803,13 +1776,13 @@
         <v>19</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D46" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
@@ -1817,13 +1790,13 @@
         <v>19</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D47" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
@@ -1831,13 +1804,13 @@
         <v>19</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="D48" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
@@ -1845,13 +1818,13 @@
         <v>19</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D49" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
@@ -1859,13 +1832,13 @@
         <v>19</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="D50" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
@@ -1873,13 +1846,13 @@
         <v>19</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D51" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
@@ -1887,13 +1860,13 @@
         <v>19</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D52" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
@@ -1901,13 +1874,13 @@
         <v>19</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="D53" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
@@ -1915,13 +1888,13 @@
         <v>19</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="D54" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
@@ -1929,13 +1902,13 @@
         <v>19</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="D55" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
@@ -1943,13 +1916,13 @@
         <v>19</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="D56" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
@@ -1957,13 +1930,13 @@
         <v>19</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="D57" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
@@ -1971,13 +1944,13 @@
         <v>19</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="D58" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
@@ -1985,13 +1958,13 @@
         <v>19</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="D59" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
@@ -1999,13 +1972,13 @@
         <v>19</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D60" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
@@ -2013,13 +1986,13 @@
         <v>19</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="D61" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
@@ -2027,13 +2000,13 @@
         <v>19</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>91</v>
+        <v>62</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>91</v>
+        <v>62</v>
       </c>
       <c r="D62" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
@@ -2041,13 +2014,13 @@
         <v>19</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D63" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
@@ -2055,13 +2028,13 @@
         <v>19</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D64" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
@@ -2069,13 +2042,13 @@
         <v>19</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="D65" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
@@ -2083,13 +2056,13 @@
         <v>19</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>95</v>
+        <v>119</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>95</v>
+        <v>119</v>
       </c>
       <c r="D66" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
@@ -2097,13 +2070,13 @@
         <v>19</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D67" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
@@ -2111,13 +2084,13 @@
         <v>19</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="D68" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
@@ -2125,13 +2098,13 @@
         <v>19</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="D69" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
@@ -2139,13 +2112,13 @@
         <v>19</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="D70" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
@@ -2153,13 +2126,13 @@
         <v>19</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D71" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
@@ -2167,13 +2140,13 @@
         <v>19</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D72" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
@@ -2181,13 +2154,13 @@
         <v>19</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="D73" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
@@ -2195,13 +2168,13 @@
         <v>19</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D74" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
@@ -2209,13 +2182,13 @@
         <v>19</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D75" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
@@ -2223,13 +2196,13 @@
         <v>19</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="D76" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
@@ -2237,13 +2210,13 @@
         <v>19</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="D77" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
@@ -2251,13 +2224,13 @@
         <v>19</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="D78" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
@@ -2265,13 +2238,13 @@
         <v>19</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D79" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
@@ -2279,13 +2252,13 @@
         <v>19</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="D80" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
@@ -2293,13 +2266,13 @@
         <v>19</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="D81" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
@@ -2307,13 +2280,13 @@
         <v>19</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="D82" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
@@ -2321,13 +2294,13 @@
         <v>19</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D83" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
@@ -2335,13 +2308,13 @@
         <v>19</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="D84" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
@@ -2349,13 +2322,13 @@
         <v>19</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="D85" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
@@ -2363,13 +2336,13 @@
         <v>19</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="D86" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
@@ -2377,13 +2350,13 @@
         <v>19</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="D87" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
@@ -2391,13 +2364,13 @@
         <v>19</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="D88" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
@@ -2405,13 +2378,13 @@
         <v>19</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D89" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
@@ -2419,13 +2392,13 @@
         <v>19</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="D90" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
@@ -2433,13 +2406,13 @@
         <v>19</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D91" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
@@ -2447,13 +2420,13 @@
         <v>19</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>121</v>
+        <v>97</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>121</v>
+        <v>97</v>
       </c>
       <c r="D92" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
@@ -2461,13 +2434,13 @@
         <v>19</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>122</v>
+        <v>94</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>122</v>
+        <v>94</v>
       </c>
       <c r="D93" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
@@ -2475,13 +2448,13 @@
         <v>19</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="D94" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
@@ -2491,7 +2464,7 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B96" s="4">
         <v>101</v>
@@ -2500,12 +2473,12 @@
         <v>101</v>
       </c>
       <c r="E96" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B97" s="4">
         <v>102</v>
@@ -2514,12 +2487,12 @@
         <v>102</v>
       </c>
       <c r="E97" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B98" s="4">
         <v>103</v>
@@ -2528,12 +2501,12 @@
         <v>103</v>
       </c>
       <c r="E98" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B99" s="4">
         <v>104</v>
@@ -2542,12 +2515,12 @@
         <v>104</v>
       </c>
       <c r="E99" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B100" s="4">
         <v>105</v>
@@ -2556,12 +2529,12 @@
         <v>105</v>
       </c>
       <c r="E100" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B101" s="4">
         <v>106</v>
@@ -2570,12 +2543,12 @@
         <v>106</v>
       </c>
       <c r="E101" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B102" s="4">
         <v>107</v>
@@ -2584,12 +2557,12 @@
         <v>107</v>
       </c>
       <c r="E102" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B103" s="4">
         <v>108</v>
@@ -2598,12 +2571,12 @@
         <v>108</v>
       </c>
       <c r="E103" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B104" s="4">
         <v>109</v>
@@ -2612,12 +2585,12 @@
         <v>109</v>
       </c>
       <c r="E104" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B105" s="4">
         <v>110</v>
@@ -2626,12 +2599,12 @@
         <v>110</v>
       </c>
       <c r="E105" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B106" s="4">
         <v>111</v>
@@ -2640,12 +2613,12 @@
         <v>111</v>
       </c>
       <c r="E106" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B107" s="4">
         <v>112</v>
@@ -2654,12 +2627,12 @@
         <v>112</v>
       </c>
       <c r="E107" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B108" s="4">
         <v>113</v>
@@ -2668,12 +2641,12 @@
         <v>113</v>
       </c>
       <c r="E108" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B109" s="4">
         <v>114</v>
@@ -2682,12 +2655,12 @@
         <v>114</v>
       </c>
       <c r="E109" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B110" s="4">
         <v>115</v>
@@ -2696,12 +2669,12 @@
         <v>115</v>
       </c>
       <c r="E110" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B111" s="4">
         <v>116</v>
@@ -2710,12 +2683,12 @@
         <v>116</v>
       </c>
       <c r="E111" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B112" s="4">
         <v>117</v>
@@ -2724,12 +2697,12 @@
         <v>117</v>
       </c>
       <c r="E112" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B113" s="4">
         <v>118</v>
@@ -2738,12 +2711,12 @@
         <v>118</v>
       </c>
       <c r="E113" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B114" s="4">
         <v>119</v>
@@ -2752,12 +2725,12 @@
         <v>119</v>
       </c>
       <c r="E114" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B115" s="4">
         <v>120</v>
@@ -2766,12 +2739,12 @@
         <v>120</v>
       </c>
       <c r="E115" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B116" s="4">
         <v>121</v>
@@ -2780,12 +2753,12 @@
         <v>121</v>
       </c>
       <c r="E116" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B117" s="4">
         <v>122</v>
@@ -2794,12 +2767,12 @@
         <v>122</v>
       </c>
       <c r="E117" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B118" s="4">
         <v>123</v>
@@ -2808,12 +2781,12 @@
         <v>123</v>
       </c>
       <c r="E118" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B119" s="4">
         <v>124</v>
@@ -2822,12 +2795,12 @@
         <v>124</v>
       </c>
       <c r="E119" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B120" s="4">
         <v>125</v>
@@ -2836,12 +2809,12 @@
         <v>125</v>
       </c>
       <c r="E120" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B121" s="4">
         <v>126</v>
@@ -2850,12 +2823,12 @@
         <v>126</v>
       </c>
       <c r="E121" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B122" s="4">
         <v>127</v>
@@ -2864,12 +2837,12 @@
         <v>127</v>
       </c>
       <c r="E122" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B123" s="4">
         <v>128</v>
@@ -2878,12 +2851,12 @@
         <v>128</v>
       </c>
       <c r="E123" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B124" s="4">
         <v>129</v>
@@ -2892,12 +2865,12 @@
         <v>129</v>
       </c>
       <c r="E124" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B125" s="4">
         <v>130</v>
@@ -2906,12 +2879,12 @@
         <v>130</v>
       </c>
       <c r="E125" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B126" s="4">
         <v>201</v>
@@ -2920,12 +2893,12 @@
         <v>201</v>
       </c>
       <c r="E126" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B127" s="4">
         <v>202</v>
@@ -2934,12 +2907,12 @@
         <v>202</v>
       </c>
       <c r="E127" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B128" s="4">
         <v>203</v>
@@ -2948,12 +2921,12 @@
         <v>203</v>
       </c>
       <c r="E128" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B129" s="4">
         <v>204</v>
@@ -2962,12 +2935,12 @@
         <v>204</v>
       </c>
       <c r="E129" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B130" s="4">
         <v>205</v>
@@ -2976,12 +2949,12 @@
         <v>205</v>
       </c>
       <c r="E130" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B131" s="4">
         <v>206</v>
@@ -2990,12 +2963,12 @@
         <v>206</v>
       </c>
       <c r="E131" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B132" s="4">
         <v>207</v>
@@ -3004,12 +2977,12 @@
         <v>207</v>
       </c>
       <c r="E132" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B133" s="4">
         <v>208</v>
@@ -3018,12 +2991,12 @@
         <v>208</v>
       </c>
       <c r="E133" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B134" s="4">
         <v>209</v>
@@ -3032,12 +3005,12 @@
         <v>209</v>
       </c>
       <c r="E134" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B135" s="4">
         <v>210</v>
@@ -3046,12 +3019,12 @@
         <v>210</v>
       </c>
       <c r="E135" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B136" s="4">
         <v>211</v>
@@ -3060,12 +3033,12 @@
         <v>211</v>
       </c>
       <c r="E136" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B137" s="4">
         <v>212</v>
@@ -3074,12 +3047,12 @@
         <v>212</v>
       </c>
       <c r="E137" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B138" s="4">
         <v>213</v>
@@ -3088,12 +3061,12 @@
         <v>213</v>
       </c>
       <c r="E138" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B139" s="4">
         <v>214</v>
@@ -3102,12 +3075,12 @@
         <v>214</v>
       </c>
       <c r="E139" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B140" s="4">
         <v>215</v>
@@ -3116,12 +3089,12 @@
         <v>215</v>
       </c>
       <c r="E140" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B141" s="4">
         <v>216</v>
@@ -3130,12 +3103,12 @@
         <v>216</v>
       </c>
       <c r="E141" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B142" s="4">
         <v>217</v>
@@ -3144,12 +3117,12 @@
         <v>217</v>
       </c>
       <c r="E142" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B143" s="4">
         <v>218</v>
@@ -3158,12 +3131,12 @@
         <v>218</v>
       </c>
       <c r="E143" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B144" s="4">
         <v>219</v>
@@ -3172,12 +3145,12 @@
         <v>219</v>
       </c>
       <c r="E144" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B145" s="4">
         <v>220</v>
@@ -3186,12 +3159,12 @@
         <v>220</v>
       </c>
       <c r="E145" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B146" s="4">
         <v>221</v>
@@ -3200,12 +3173,12 @@
         <v>221</v>
       </c>
       <c r="E146" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B147" s="4">
         <v>222</v>
@@ -3214,12 +3187,12 @@
         <v>222</v>
       </c>
       <c r="E147" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A148" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B148" s="4">
         <v>223</v>
@@ -3228,12 +3201,12 @@
         <v>223</v>
       </c>
       <c r="E148" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A149" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B149" s="4">
         <v>224</v>
@@ -3242,12 +3215,12 @@
         <v>224</v>
       </c>
       <c r="E149" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A150" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B150" s="4">
         <v>225</v>
@@ -3256,12 +3229,12 @@
         <v>225</v>
       </c>
       <c r="E150" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A151" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B151" s="4">
         <v>226</v>
@@ -3270,12 +3243,12 @@
         <v>226</v>
       </c>
       <c r="E151" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A152" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B152" s="4">
         <v>227</v>
@@ -3284,12 +3257,12 @@
         <v>227</v>
       </c>
       <c r="E152" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A153" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B153" s="4">
         <v>228</v>
@@ -3298,12 +3271,12 @@
         <v>228</v>
       </c>
       <c r="E153" t="s">
-        <v>91</v>
+        <v>62</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A154" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B154" s="4">
         <v>229</v>
@@ -3312,12 +3285,12 @@
         <v>229</v>
       </c>
       <c r="E154" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A155" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B155" s="4">
         <v>230</v>
@@ -3326,12 +3299,12 @@
         <v>230</v>
       </c>
       <c r="E155" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A156" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B156" s="4">
         <v>301</v>
@@ -3340,12 +3313,12 @@
         <v>301</v>
       </c>
       <c r="E156" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A157" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B157" s="4">
         <v>302</v>
@@ -3354,12 +3327,12 @@
         <v>302</v>
       </c>
       <c r="E157" t="s">
-        <v>95</v>
+        <v>119</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A158" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B158" s="4">
         <v>303</v>
@@ -3368,12 +3341,12 @@
         <v>303</v>
       </c>
       <c r="E158" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A159" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B159" s="4">
         <v>304</v>
@@ -3382,12 +3355,12 @@
         <v>304</v>
       </c>
       <c r="E159" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A160" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B160" s="4">
         <v>305</v>
@@ -3396,12 +3369,12 @@
         <v>305</v>
       </c>
       <c r="E160" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A161" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B161" s="4">
         <v>306</v>
@@ -3410,12 +3383,12 @@
         <v>306</v>
       </c>
       <c r="E161" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A162" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B162" s="4">
         <v>307</v>
@@ -3424,12 +3397,12 @@
         <v>307</v>
       </c>
       <c r="E162" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A163" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B163" s="4">
         <v>308</v>
@@ -3438,12 +3411,12 @@
         <v>308</v>
       </c>
       <c r="E163" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A164" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B164" s="4">
         <v>309</v>
@@ -3452,12 +3425,12 @@
         <v>309</v>
       </c>
       <c r="E164" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A165" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B165" s="4">
         <v>310</v>
@@ -3466,12 +3439,12 @@
         <v>310</v>
       </c>
       <c r="E165" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A166" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B166" s="4">
         <v>311</v>
@@ -3480,12 +3453,12 @@
         <v>311</v>
       </c>
       <c r="E166" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A167" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B167" s="4">
         <v>312</v>
@@ -3494,12 +3467,12 @@
         <v>312</v>
       </c>
       <c r="E167" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A168" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B168" s="4">
         <v>313</v>
@@ -3508,12 +3481,12 @@
         <v>313</v>
       </c>
       <c r="E168" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A169" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B169" s="4">
         <v>314</v>
@@ -3522,12 +3495,12 @@
         <v>314</v>
       </c>
       <c r="E169" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A170" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B170" s="4">
         <v>315</v>
@@ -3536,12 +3509,12 @@
         <v>315</v>
       </c>
       <c r="E170" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A171" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B171" s="4">
         <v>316</v>
@@ -3550,12 +3523,12 @@
         <v>316</v>
       </c>
       <c r="E171" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A172" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B172" s="4">
         <v>317</v>
@@ -3564,12 +3537,12 @@
         <v>317</v>
       </c>
       <c r="E172" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A173" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B173" s="4">
         <v>318</v>
@@ -3578,12 +3551,12 @@
         <v>318</v>
       </c>
       <c r="E173" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A174" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B174" s="4">
         <v>319</v>
@@ -3592,12 +3565,12 @@
         <v>319</v>
       </c>
       <c r="E174" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A175" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B175" s="4">
         <v>320</v>
@@ -3606,12 +3579,12 @@
         <v>320</v>
       </c>
       <c r="E175" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A176" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B176" s="4">
         <v>321</v>
@@ -3620,12 +3593,12 @@
         <v>321</v>
       </c>
       <c r="E176" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A177" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B177" s="4">
         <v>322</v>
@@ -3634,12 +3607,12 @@
         <v>322</v>
       </c>
       <c r="E177" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A178" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B178" s="4">
         <v>323</v>
@@ -3648,12 +3621,12 @@
         <v>323</v>
       </c>
       <c r="E178" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A179" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B179" s="4">
         <v>324</v>
@@ -3662,12 +3635,12 @@
         <v>324</v>
       </c>
       <c r="E179" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A180" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B180" s="4">
         <v>325</v>
@@ -3676,12 +3649,12 @@
         <v>325</v>
       </c>
       <c r="E180" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A181" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B181" s="4">
         <v>326</v>
@@ -3690,12 +3663,12 @@
         <v>326</v>
       </c>
       <c r="E181" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A182" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B182" s="4">
         <v>327</v>
@@ -3704,12 +3677,12 @@
         <v>327</v>
       </c>
       <c r="E182" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A183" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B183" s="4">
         <v>328</v>
@@ -3718,12 +3691,12 @@
         <v>328</v>
       </c>
       <c r="E183" t="s">
-        <v>121</v>
+        <v>97</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A184" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B184" s="4">
         <v>329</v>
@@ -3732,12 +3705,12 @@
         <v>329</v>
       </c>
       <c r="E184" t="s">
-        <v>122</v>
+        <v>94</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A185" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B185" s="4">
         <v>330</v>
@@ -3746,7 +3719,7 @@
         <v>330</v>
       </c>
       <c r="E185" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.2">
@@ -4150,7 +4123,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4178,16 +4151,16 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>29</v>
+        <v>146</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>27</v>
+        <v>145</v>
       </c>
       <c r="C2">
         <v>20210224</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E2" s="3"/>
     </row>

</xml_diff>